<commit_message>
Shipping information Page coded added
</commit_message>
<xml_diff>
--- a/src/main/java/com/aakash/qa/testdata/AakashProjectData.xlsx
+++ b/src/main/java/com/aakash/qa/testdata/AakashProjectData.xlsx
@@ -5,18 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\010645_puresoft\Desktop\Desktop\Work\Selenium Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\010645_puresoft\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A41E4BB-CCFB-4D79-AC93-FD34815734AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D65F434-F999-49E0-B857-AB0280386271}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5B58FED1-E6F3-4CCE-966B-CB97FC14D8F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Eng" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
-    <sheet name="Medical" sheetId="2" r:id="rId3"/>
-    <sheet name="Foundation" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="5" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
+    <sheet name="Medical" sheetId="2" r:id="rId4"/>
+    <sheet name="Foundation" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
   <si>
     <t>State</t>
   </si>
@@ -85,13 +86,52 @@
   </si>
   <si>
     <t>Pandey</t>
+  </si>
+  <si>
+    <t>Parent name</t>
+  </si>
+  <si>
+    <t>parent mobile</t>
+  </si>
+  <si>
+    <t>parent email</t>
+  </si>
+  <si>
+    <t>streetAddress</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>pin code</t>
+  </si>
+  <si>
+    <t>Shiping_state</t>
+  </si>
+  <si>
+    <t>9560370108</t>
+  </si>
+  <si>
+    <t>Ak Pandey</t>
+  </si>
+  <si>
+    <t>arunpandey.pus@aesl.in</t>
+  </si>
+  <si>
+    <t>JKHouse- Plot 32 Pusa road</t>
+  </si>
+  <si>
+    <t>Noida</t>
+  </si>
+  <si>
+    <t>Uttar Pradesh</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -99,8 +139,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -110,6 +158,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -138,10 +192,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -167,8 +222,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -481,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6473CB0D-1CBA-4422-BE1A-F0DE286CDFB4}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E2"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -492,10 +552,18 @@
     <col min="1" max="1" width="12.26953125" style="3" customWidth="1"/>
     <col min="2" max="2" width="16.54296875" style="3" customWidth="1"/>
     <col min="3" max="3" width="21.90625" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="8.7265625" style="3"/>
+    <col min="4" max="4" width="9.7265625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="11.36328125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="11.453125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="15.54296875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="18.7265625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="22.90625" style="3" customWidth="1"/>
+    <col min="10" max="11" width="8.7265625" style="3"/>
+    <col min="12" max="12" width="11.7265625" style="3" customWidth="1"/>
+    <col min="13" max="16384" width="8.7265625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>1</v>
       </c>
@@ -511,8 +579,29 @@
       <c r="E1" s="9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F1" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
@@ -528,14 +617,163 @@
       <c r="E2" s="10" t="s">
         <v>16</v>
       </c>
+      <c r="F2" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="K2" s="13">
+        <v>201305</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>29</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{5E63A2B8-4D1A-4CF9-8B50-B56F16F23A09}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D272B0E4-503E-44CC-ABEE-A172C2BA137C}">
+  <dimension ref="I6:K24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K6" sqref="K6:K24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="6" spans="9:11" x14ac:dyDescent="0.35">
+      <c r="K6">
+        <v>17700</v>
+      </c>
+    </row>
+    <row r="7" spans="9:11" x14ac:dyDescent="0.35">
+      <c r="K7">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="9:11" x14ac:dyDescent="0.35">
+      <c r="K8">
+        <v>11900</v>
+      </c>
+    </row>
+    <row r="9" spans="9:11" x14ac:dyDescent="0.35">
+      <c r="I9">
+        <v>14160</v>
+      </c>
+      <c r="K9">
+        <v>5650</v>
+      </c>
+    </row>
+    <row r="10" spans="9:11" x14ac:dyDescent="0.35">
+      <c r="I10">
+        <v>8240</v>
+      </c>
+      <c r="K10">
+        <v>11843</v>
+      </c>
+    </row>
+    <row r="11" spans="9:11" x14ac:dyDescent="0.35">
+      <c r="I11">
+        <v>2126</v>
+      </c>
+      <c r="K11">
+        <v>4522</v>
+      </c>
+    </row>
+    <row r="12" spans="9:11" x14ac:dyDescent="0.35">
+      <c r="I12">
+        <v>1434</v>
+      </c>
+      <c r="K12">
+        <v>2975</v>
+      </c>
+    </row>
+    <row r="13" spans="9:11" x14ac:dyDescent="0.35">
+      <c r="I13">
+        <v>19832</v>
+      </c>
+      <c r="K13">
+        <v>23324</v>
+      </c>
+    </row>
+    <row r="14" spans="9:11" x14ac:dyDescent="0.35">
+      <c r="K14">
+        <v>5950</v>
+      </c>
+    </row>
+    <row r="15" spans="9:11" x14ac:dyDescent="0.35">
+      <c r="K15">
+        <v>3987</v>
+      </c>
+    </row>
+    <row r="16" spans="9:11" x14ac:dyDescent="0.35">
+      <c r="K16">
+        <v>29155</v>
+      </c>
+    </row>
+    <row r="17" spans="11:11" x14ac:dyDescent="0.35">
+      <c r="K17">
+        <v>7497</v>
+      </c>
+    </row>
+    <row r="18" spans="11:11" x14ac:dyDescent="0.35">
+      <c r="K18">
+        <v>4998</v>
+      </c>
+    </row>
+    <row r="19" spans="11:11" x14ac:dyDescent="0.35">
+      <c r="K19">
+        <v>23324</v>
+      </c>
+    </row>
+    <row r="20" spans="11:11" x14ac:dyDescent="0.35">
+      <c r="K20">
+        <v>5950</v>
+      </c>
+    </row>
+    <row r="21" spans="11:11" x14ac:dyDescent="0.35">
+      <c r="K21">
+        <v>3987</v>
+      </c>
+    </row>
+    <row r="22" spans="11:11" x14ac:dyDescent="0.35">
+      <c r="K22">
+        <v>23324</v>
+      </c>
+    </row>
+    <row r="23" spans="11:11" x14ac:dyDescent="0.35">
+      <c r="K23">
+        <v>5950</v>
+      </c>
+    </row>
+    <row r="24" spans="11:11" x14ac:dyDescent="0.35">
+      <c r="K24">
+        <v>3987</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5055F819-850C-4283-A3CD-25AFD65FB96A}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -572,7 +810,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8953C48-4B6B-4BD5-B7F0-C7F1612DCDCF}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -614,7 +852,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BB2E982-2451-4DB0-94FF-AADF13FE2CD0}">
   <dimension ref="A1:C2"/>
   <sheetViews>

</xml_diff>

<commit_message>
code added for Shipping Frame
</commit_message>
<xml_diff>
--- a/src/main/java/com/aakash/qa/testdata/AakashProjectData.xlsx
+++ b/src/main/java/com/aakash/qa/testdata/AakashProjectData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\010645_puresoft\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D65F434-F999-49E0-B857-AB0280386271}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EEFCB1F-E8F9-454B-9740-BFA0113F6210}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5B58FED1-E6F3-4CCE-966B-CB97FC14D8F0}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
   <si>
     <t>State</t>
   </si>
@@ -125,6 +125,9 @@
   </si>
   <si>
     <t>Uttar Pradesh</t>
+  </si>
+  <si>
+    <t>201305</t>
   </si>
 </sst>
 </file>
@@ -543,7 +546,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6473CB0D-1CBA-4422-BE1A-F0DE286CDFB4}">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
@@ -632,8 +635,8 @@
       <c r="J2" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="K2" s="13">
-        <v>201305</v>
+      <c r="K2" s="13" t="s">
+        <v>30</v>
       </c>
       <c r="L2" s="13" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
clear field and explicit wait code added for dataprovider test
</commit_message>
<xml_diff>
--- a/src/main/java/com/aakash/qa/testdata/AakashProjectData.xlsx
+++ b/src/main/java/com/aakash/qa/testdata/AakashProjectData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\010645_puresoft\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EEFCB1F-E8F9-454B-9740-BFA0113F6210}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7917C7E8-D90E-41A8-A808-3E1CD7B6F12D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5B58FED1-E6F3-4CCE-966B-CB97FC14D8F0}"/>
   </bookViews>
@@ -199,7 +199,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -224,7 +224,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -547,7 +546,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -582,25 +581,25 @@
       <c r="E1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="L1" s="10" t="s">
         <v>23</v>
       </c>
     </row>
@@ -614,31 +613,31 @@
       <c r="C2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="J2" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="K2" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="L2" s="12" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>